<commit_message>
feat: menambahkan file pdf dari file excel soal 2 nf dan 3 nf
</commit_message>
<xml_diff>
--- a/task-w9d1/nf.xlsx
+++ b/task-w9d1/nf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/53fa144662bcffb8/Documents/Courses/Bootcamp - Koda/week-9/tasks-w9/task-w9d1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="140" documentId="8_{AA3494C6-B05F-4BE0-93DD-6C0BC19F91CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E8A78C9-7D33-46D9-9063-810680B1EA3C}"/>
+  <xr:revisionPtr revIDLastSave="162" documentId="8_{AA3494C6-B05F-4BE0-93DD-6C0BC19F91CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{16A8793B-014D-424C-B40D-937DBEFB2514}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{A87ABF1F-00B5-474C-B98C-952061D666EF}"/>
   </bookViews>
@@ -139,7 +139,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,6 +157,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -188,7 +196,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -224,17 +232,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -251,10 +265,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -669,10 +687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E573A2E8-D953-48D0-A91F-96E7F80D0288}">
-  <dimension ref="A6:K64"/>
+  <dimension ref="A6:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="D1" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -690,623 +708,618 @@
     <col min="13" max="13" width="9.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="10" t="s">
+    <row r="6" spans="1:11" ht="26" x14ac:dyDescent="0.6">
+      <c r="B6" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="J7" s="5" t="s">
         <v>8</v>
       </c>
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="4">
         <v>45200</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="4">
         <v>45214</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J8" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="4">
         <v>45201</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="4">
         <v>45215</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="J9" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="4">
         <v>45204</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="4">
         <v>45218</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="J10" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="4">
         <v>45209</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="4">
         <v>45223</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="J11" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B13" s="11" t="s">
+    <row r="14" spans="1:11" ht="26" x14ac:dyDescent="0.6">
+      <c r="B14" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B14" s="8" t="s">
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="9"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B15" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C15" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D15" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F15" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G15" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="H15" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="I15" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B15" s="4" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B16" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F16" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G16" s="4">
         <v>45200</v>
       </c>
-      <c r="H15" s="5">
+      <c r="H16" s="4">
         <v>45214</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="I16" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B16" s="4" t="s">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B17" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D17" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F17" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G17" s="4">
         <v>45201</v>
       </c>
-      <c r="H16" s="5">
+      <c r="H17" s="4">
         <v>45215</v>
       </c>
-      <c r="I16" s="4" t="s">
+      <c r="I17" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B17" s="4" t="s">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B18" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D18" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F18" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G17" s="5">
+      <c r="G18" s="4">
         <v>45204</v>
       </c>
-      <c r="H17" s="5">
+      <c r="H18" s="4">
         <v>45218</v>
       </c>
-      <c r="I17" s="4" t="s">
+      <c r="I18" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B18" s="4" t="s">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B19" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D19" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F19" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G19" s="4">
         <v>45209</v>
       </c>
-      <c r="H18" s="5">
+      <c r="H19" s="4">
         <v>45223</v>
       </c>
-      <c r="I18" s="4" t="s">
+      <c r="I19" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B20" s="8" t="s">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B21" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C21" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F21" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G20" s="8" t="s">
+      <c r="G21" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H20" s="8" t="s">
+      <c r="H21" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B21" s="4" t="s">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B22" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F22" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="G22" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H21" s="4" t="s">
+      <c r="H22" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B22" s="4" t="s">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B23" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C23" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="F23" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="G23" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H22" s="4" t="s">
+      <c r="H23" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B23" s="4" t="s">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B24" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C24" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="F24" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="G24" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H23" s="4" t="s">
+      <c r="H24" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B24" s="4" t="s">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B25" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C25" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="F25" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G24" s="4" t="s">
+      <c r="G25" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H24" s="4" t="s">
+      <c r="H25" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B39" t="s">
+    <row r="28" spans="2:9" ht="26" x14ac:dyDescent="0.6">
+      <c r="B28" s="10" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B40" s="7" t="s">
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B29" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="C29" s="6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B41" s="4">
+      <c r="E29" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B30" s="3">
         <v>1</v>
       </c>
-      <c r="C41" s="9" t="s">
+      <c r="C30" s="8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B42" s="4">
+      <c r="E30" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F30" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B31" s="3">
         <v>2</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C31" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B43" s="4">
+      <c r="E31" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F31" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B32" s="3">
         <v>3</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C32" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B45" s="7" t="s">
+      <c r="E32" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B34" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="C34" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B46" s="4" t="s">
+      <c r="E34" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B35" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C35" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B47" s="4" t="s">
+      <c r="E35" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B36" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C36" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B48" s="4" t="s">
+      <c r="E36" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B37" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C37" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B51" s="3" t="s">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B39" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C51" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B52" s="4" t="s">
+      <c r="D39" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B40" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C52" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B53" s="4" t="s">
+      <c r="D40" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="4">
+        <v>45200</v>
+      </c>
+      <c r="F40" s="4">
+        <v>45214</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B41" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C53" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B54" s="4" t="s">
+      <c r="D41" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" s="4">
+        <v>45201</v>
+      </c>
+      <c r="F41" s="4">
+        <v>45215</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B42" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C54" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B56" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B57" s="4" t="s">
+      <c r="D42" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" s="4">
+        <v>45204</v>
+      </c>
+      <c r="F42" s="4">
+        <v>45218</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B43" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C57" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B58" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B60" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C60" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D60" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E60" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F60" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G60" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B61" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D61" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E61" s="5">
-        <v>45200</v>
-      </c>
-      <c r="F61" s="5">
-        <v>45214</v>
-      </c>
-      <c r="G61" s="4" t="s">
+      <c r="C43" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E43" s="4">
+        <v>45209</v>
+      </c>
+      <c r="F43" s="4">
+        <v>45223</v>
+      </c>
+      <c r="G43" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B62" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D62" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E62" s="5">
-        <v>45201</v>
-      </c>
-      <c r="F62" s="5">
-        <v>45215</v>
-      </c>
-      <c r="G62" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B63" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D63" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E63" s="5">
-        <v>45204</v>
-      </c>
-      <c r="F63" s="5">
-        <v>45218</v>
-      </c>
-      <c r="G63" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B64" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D64" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E64" s="5">
-        <v>45209</v>
-      </c>
-      <c r="F64" s="5">
-        <v>45223</v>
-      </c>
-      <c r="G64" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="B13:J13"/>
+  <mergeCells count="3">
+    <mergeCell ref="B28:I28"/>
+    <mergeCell ref="B14:I14"/>
+    <mergeCell ref="B6:J6"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="C41:C43 C45">
+  <conditionalFormatting sqref="C30:C32 C34">
     <cfRule type="duplicateValues" dxfId="3" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C52:C54">
+  <conditionalFormatting sqref="F30:F32">
     <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H21:H23">
-    <cfRule type="duplicateValues" dxfId="1" priority="4"/>
+  <conditionalFormatting sqref="G8:G10">
+    <cfRule type="duplicateValues" dxfId="1" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G8:G10">
-    <cfRule type="duplicateValues" dxfId="0" priority="7"/>
+  <conditionalFormatting sqref="H22:H24">
+    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" scale="72" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>